<commit_message>
Deploying to gh-pages from  @ f503c3049389b9a99cc6791362820524408d681b 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.xlsx
+++ b/en/downloads/data-excel/1.1.1.xlsx
@@ -712,10 +712,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,7 +735,7 @@
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1">
+    <row r="1" spans="1:19" ht="30" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="19.5" customHeight="1">
+    <row r="2" spans="1:19" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -777,7 +777,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:19" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -792,7 +792,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -847,8 +847,11 @@
       <c r="R4" s="14">
         <v>2021</v>
       </c>
+      <c r="S4" s="14">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1">
+    <row r="5" spans="1:19" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
@@ -903,8 +906,11 @@
       <c r="R5" s="29">
         <v>8.0841202038693286E-2</v>
       </c>
+      <c r="S5" s="29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
@@ -959,8 +965,11 @@
       <c r="R6" s="30">
         <v>0</v>
       </c>
+      <c r="S6" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1">
+    <row r="7" spans="1:19" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
@@ -1015,8 +1024,11 @@
       <c r="R7" s="30">
         <v>0</v>
       </c>
+      <c r="S7" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1">
+    <row r="8" spans="1:19" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -1071,8 +1083,11 @@
       <c r="R8" s="30">
         <v>0</v>
       </c>
+      <c r="S8" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1">
+    <row r="9" spans="1:19" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1127,8 +1142,11 @@
       <c r="R9" s="30">
         <v>0.2462269049859406</v>
       </c>
+      <c r="S9" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1">
+    <row r="10" spans="1:19" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
@@ -1183,8 +1201,11 @@
       <c r="R10" s="30">
         <v>0</v>
       </c>
+      <c r="S10" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1">
+    <row r="11" spans="1:19" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
@@ -1239,8 +1260,11 @@
       <c r="R11" s="30">
         <v>0</v>
       </c>
+      <c r="S11" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1">
+    <row r="12" spans="1:19" ht="15.75" customHeight="1">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -1295,8 +1319,11 @@
       <c r="R12" s="30">
         <v>0</v>
       </c>
+      <c r="S12" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" s="25" t="s">
         <v>26</v>
       </c>
@@ -1351,8 +1378,11 @@
       <c r="R13" s="30">
         <v>0</v>
       </c>
+      <c r="S13" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1">
+    <row r="14" spans="1:19" ht="15.75" thickBot="1">
       <c r="A14" s="26" t="s">
         <v>28</v>
       </c>
@@ -1397,6 +1427,9 @@
       <c r="R14" s="10">
         <v>1.4177257229737372</v>
       </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>